<commit_message>
revised bar chart figure; updating file mgmt
</commit_message>
<xml_diff>
--- a/NRCS-synonyms.xlsx
+++ b/NRCS-synonyms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/stefanie_lane_ubc_ca/Documents/Documents/Dissertation/CommunityStability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\CommunityStability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BBCA418-9FA3-4D0D-97DC-5641F3A63B93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4BBCA418-9FA3-4D0D-97DC-5641F3A63B93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{86EA6625-AF84-4DA1-813C-94693BCF1A0B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NRCS_synonyms" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="244">
   <si>
     <t>NRCS</t>
   </si>
@@ -586,9 +586,6 @@
   </si>
   <si>
     <t>Poaceae_misc</t>
-  </si>
-  <si>
-    <t>GATR3</t>
   </si>
   <si>
     <t>Rumex_conglomeratus</t>
@@ -1306,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE52639D-E8F1-4773-B74D-3E40B131B609}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1329,10 +1326,10 @@
         <v>2019</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1354,32 +1351,32 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="22" t="s">
@@ -1389,14 +1386,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="20"/>
     </row>
@@ -1433,7 +1430,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="16" t="s">
@@ -1444,7 +1441,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="17" t="s">
@@ -1484,25 +1481,25 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E14" s="20"/>
     </row>
@@ -1549,27 +1546,27 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19" s="23"/>
     </row>
@@ -1590,12 +1587,12 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21" s="23"/>
     </row>
@@ -1612,14 +1609,14 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="26" t="s">
         <v>83</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>178</v>
+        <v>84</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>49</v>
@@ -1628,7 +1625,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="17" t="s">
@@ -1651,14 +1648,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E26" s="20"/>
     </row>
@@ -1691,10 +1688,10 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>80</v>
@@ -1772,38 +1769,38 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E36" s="20"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E37" s="23"/>
     </row>
@@ -1811,20 +1808,20 @@
       <c r="A38" s="11"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E38" s="20"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>174</v>
@@ -1863,10 +1860,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>46</v>
@@ -1910,12 +1907,12 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="26"/>
       <c r="D45" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E45" s="23"/>
     </row>
@@ -1932,13 +1929,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>130</v>
@@ -1947,14 +1944,14 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E48" s="20"/>
     </row>
@@ -1990,32 +1987,32 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="24"/>
       <c r="D52" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E52" s="20"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="8"/>
       <c r="B53" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="16" t="s">
@@ -2025,12 +2022,12 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
       <c r="D54" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E54" s="20"/>
     </row>
@@ -2051,12 +2048,12 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
       <c r="D56" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E56" s="20"/>
     </row>
@@ -2066,7 +2063,7 @@
       </c>
       <c r="B57" s="26"/>
       <c r="C57" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>139</v>
@@ -2131,25 +2128,25 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E62" s="20"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
       <c r="D63" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E63" s="23"/>
     </row>
@@ -2166,10 +2163,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>58</v>
@@ -2183,13 +2180,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>77</v>
@@ -2198,37 +2195,37 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C67" s="26"/>
       <c r="D67" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E67" s="23"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
       <c r="D68" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E68" s="20"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D69" s="22" t="s">
         <v>60</v>
@@ -2239,13 +2236,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>36</v>
@@ -2274,7 +2271,7 @@
       <c r="B72" s="18"/>
       <c r="C72" s="18"/>
       <c r="D72" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E72" s="20"/>
     </row>
@@ -2291,9 +2288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2580,6 +2577,9 @@
       <c r="D12" t="s">
         <v>49</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="F12" t="s">
         <v>102</v>
       </c>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C23" t="s">
         <v>150</v>
@@ -3348,12 +3348,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -3582,6 +3576,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{040982B5-65AA-4C72-97AA-3A5DA879E500}">
   <ds:schemaRefs>
@@ -3591,23 +3591,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBFBA52-F9D8-4B16-8C13-5E059880ED7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D32B733-5EF8-47F5-959A-F5C14F1B9901}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3624,4 +3607,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBFBA52-F9D8-4B16-8C13-5E059880ED7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>